<commit_message>
Integrate new results from 2080Ti
</commit_message>
<xml_diff>
--- a/results/2080Ti/GraphInit.xlsx
+++ b/results/2080Ti/GraphInit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University\GPUMemManSurvey\results\2080Ti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3E1806-34A3-475A-92FF-F1EFD3333373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D96186-F7CC-436F-8612-83FE997D2726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,10 +182,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -717,6 +718,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>103.265</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9034300000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.492477</c:v>
@@ -2607,10 +2611,10 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7B9C8B1E-FFBD-4346-B249-F623197CBEA8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="304" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0"/>
-  <pageSetup paperSize="157" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -2619,7 +2623,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8873289" cy="3487278"/>
+    <xdr:ext cx="12681857" cy="7667625"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2914,7 +2918,7 @@
   <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F3" sqref="F3:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2937,22 +2941,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
@@ -3017,10 +3021,10 @@
       <c r="D3" s="3">
         <v>3.7665999999999999</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>4.6594100000000003</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <v>4.0957600000000003</v>
       </c>
       <c r="G3" s="3">
@@ -3067,10 +3071,10 @@
       <c r="D4" s="3">
         <v>66.614800000000002</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>80.061599999999999</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <v>69.555199999999999</v>
       </c>
       <c r="G4" s="3">
@@ -3111,10 +3115,10 @@
       <c r="D5" s="3">
         <v>113.21599999999999</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>127.384</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <v>103.265</v>
       </c>
       <c r="G5" s="3">
@@ -3157,8 +3161,12 @@
       <c r="D6" s="3">
         <v>1.43207</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="4">
+        <v>4.4759799999999998</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4.2688300000000003</v>
+      </c>
       <c r="G6" s="3">
         <v>0.31636500000000001</v>
       </c>
@@ -3203,10 +3211,12 @@
       <c r="D7" s="3">
         <v>1.36873</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>1.43885</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="4">
+        <v>3.9034300000000002</v>
+      </c>
       <c r="G7" s="3">
         <v>0.34344799999999998</v>
       </c>
@@ -3251,10 +3261,10 @@
       <c r="D8" s="3">
         <v>18.562899999999999</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="4">
         <v>21.970400000000001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>19.073599999999999</v>
       </c>
       <c r="G8" s="3">
@@ -3301,10 +3311,10 @@
       <c r="D9" s="3">
         <v>0.44794600000000001</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="4">
         <v>0.47951500000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>0.492477</v>
       </c>
       <c r="G9" s="3">
@@ -3349,10 +3359,10 @@
       <c r="D10" s="3">
         <v>95.59</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="4">
         <v>107.726</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="4">
         <v>88.133899999999997</v>
       </c>
       <c r="G10" s="3">
@@ -3395,10 +3405,10 @@
       <c r="D11" s="3">
         <v>1.83856</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="4">
         <v>1.95848</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <v>1.6121399999999999</v>
       </c>
       <c r="G11" s="3">
@@ -3445,10 +3455,10 @@
       <c r="D12" s="3">
         <v>1.6233299999999999</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>1.8022400000000001</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <v>1.6025799999999999</v>
       </c>
       <c r="G12" s="3">
@@ -3495,10 +3505,10 @@
       <c r="D13" s="3">
         <v>27.126300000000001</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>34.909999999999997</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="4">
         <v>28.569900000000001</v>
       </c>
       <c r="G13" s="3">
@@ -3545,10 +3555,10 @@
       <c r="D14" s="3">
         <v>1.2856300000000001</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="4">
         <v>1.3208599999999999</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="4">
         <v>1.10886</v>
       </c>
       <c r="G14" s="3">
@@ -3595,10 +3605,10 @@
       <c r="D15" s="3">
         <v>0.87265999999999999</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="4">
         <v>0.89028700000000005</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <v>0.84923300000000002</v>
       </c>
       <c r="G15" s="3">
@@ -3633,76 +3643,76 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+      <c r="Q52" s="6"/>
     </row>
     <row r="69" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B69" s="5"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-      <c r="K69" s="5"/>
-      <c r="L69" s="5"/>
-      <c r="M69" s="5"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="5"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+      <c r="N69" s="6"/>
+      <c r="O69" s="6"/>
+      <c r="P69" s="6"/>
+      <c r="Q69" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>